<commit_message>
updae en nieuwe data
Former-commit-id: 6ddbc39a781121e8d9c80325109d451262ddb076
</commit_message>
<xml_diff>
--- a/Tijdscomplexiteit algoritmen.xlsx
+++ b/Tijdscomplexiteit algoritmen.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="s &lt;= 0,01" sheetId="5" r:id="rId1"/>
-    <sheet name="s &lt;= 0,2" sheetId="1" r:id="rId2"/>
-    <sheet name="s &lt;= 0,1" sheetId="3" r:id="rId3"/>
+    <sheet name="s &lt;= 0,1" sheetId="3" r:id="rId2"/>
+    <sheet name="s &lt;= 0,2" sheetId="1" r:id="rId3"/>
     <sheet name="s &lt;= 0,5" sheetId="4" r:id="rId4"/>
     <sheet name="s &lt;= 1" sheetId="6" r:id="rId5"/>
   </sheets>
@@ -240,6 +240,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -249,6 +297,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>5.5516999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.6510999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9249000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16561899999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79310400000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2871619999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1092139999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.2961150000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.111768999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.772381000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>80.574263000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>205.43500399999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>820.38240699999994</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3289.07998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15940.149552000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>67381.763546999995</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -298,6 +394,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -307,6 +451,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1.284362</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7646999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2980999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12456399999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22673399999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29065000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.63634999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2836959999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.2044309999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0112190000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.6268189999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0782220000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.974940999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31.238512</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>102.424753</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>460.93494900000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -356,6 +548,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -365,6 +605,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1.2829630000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9715999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16142000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20200899999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.50198900000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74785000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7746869999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9979339999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.2076510000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9634330000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.2643680000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.793704999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.557507999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.914204000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>65.278081</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>225.832246</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -378,11 +666,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="346374352"/>
-        <c:axId val="346374744"/>
+        <c:axId val="353034960"/>
+        <c:axId val="353031824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="346374352"/>
+        <c:axId val="353034960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -402,6 +690,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-BE"/>
+                  <a:t>Aantal rechthoeken</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-BE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -439,12 +783,12 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346374744"/>
+        <c:crossAx val="353031824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="346374744"/>
+        <c:axId val="353031824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -465,6 +809,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-BE"/>
+                  <a:t>Tijd</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-BE" baseline="0"/>
+                  <a:t> in miliseconden</a:t>
+                </a:r>
+                <a:endParaRPr lang="nl-BE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-BE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -502,7 +907,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346374352"/>
+        <c:crossAx val="353034960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -620,875 +1025,6 @@
               <a:rPr lang="nl-BE" sz="1800" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Doubeling experiment (max. lengte zijde = 0.2) </a:t>
-            </a:r>
-            <a:endParaRPr lang="nl-BE">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'s &lt;= 0,2'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Algoritme1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'s &lt;= 0,2'!$A$2:$A$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32768</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'s &lt;= 0,2'!$B$2:$B$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
-                <c:pt idx="0">
-                  <c:v>4.7223000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.9347000000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.9225E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.35874600000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.77075300000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.4476689999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16.724685999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>64.328180000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45.292262000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>28.154897999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>89.458753999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>409.24207899999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1698.683477</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8778.2531400000007</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>36192.314450999998</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>231158.01998899999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'s &lt;= 0,2'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Algoritme2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'s &lt;= 0,2'!$A$2:$A$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32768</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'s &lt;= 0,2'!$C$2:$C$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
-                <c:pt idx="0">
-                  <c:v>1.427926</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.5888E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.8627999999999995E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.25318400000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.46081499999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.766035</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.5092669999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>17.058319000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16.253195000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14.791833</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>35.258977999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>158.16474700000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>845.33772199999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2508.9897179999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>20610.072639000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>94613.954494000005</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'s &lt;= 0,2'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Algoritme3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'s &lt;= 0,2'!$A$2:$A$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32768</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'s &lt;= 0,2'!$D$2:$D$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
-                <c:pt idx="0">
-                  <c:v>2.3958879999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.6593000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.30030099999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.67792300000000005</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8269759999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.3838950000000008</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16.409811999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>113.157793</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>82.311852999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>65.254551000000006</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>109.60528600000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>342.60131000000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1600.68336</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6551.8527519999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>32770.112476000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>160632.83349300001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="348332632"/>
-        <c:axId val="348336160"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="348332632"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="nl-BE"/>
-                  <a:t>Aantal rechthoeken</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-BE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="348336160"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="348336160"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="nl-BE"/>
-                  <a:t>Tijd</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="nl-BE" baseline="0"/>
-                  <a:t> in miliseconden</a:t>
-                </a:r>
-                <a:endParaRPr lang="nl-BE"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-BE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="348332632"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="nl-BE" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
               <a:t>Doubeling experiment (max. lengte zijde = 0.1) </a:t>
             </a:r>
             <a:endParaRPr lang="nl-BE">
@@ -1577,6 +1113,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1586,6 +1170,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>5.645E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6451000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0324E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15068999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67367200000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0622929999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6431480000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.9315090000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.048589</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>69.110174000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>76.222920000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>258.82211899999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1073.4199960000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4403.0896540000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22048.870620000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>84398.026849999995</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1635,6 +1267,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1644,6 +1324,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1.794281</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6186999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0324E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18474699999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28271800000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39375300000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.137872</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9076489999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.9419950000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.6436820000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.8930319999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29.101796</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>128.773077</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>686.64916300000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2393.8336610000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13215.184121</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1693,6 +1421,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1702,6 +1478,54 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>34.192126000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2981999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4239000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42687700000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57663399999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0319689999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5125409999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.5906960000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.9849160000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.023949</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.467199999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45.625889000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>178.02485300000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>660.72211700000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3076.5924129999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16846.653752999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1715,11 +1539,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="348336552"/>
-        <c:axId val="348337336"/>
+        <c:axId val="120001096"/>
+        <c:axId val="358811192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="348336552"/>
+        <c:axId val="120001096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1832,12 +1656,12 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348337336"/>
+        <c:crossAx val="358811192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="348337336"/>
+        <c:axId val="358811192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1956,7 +1780,880 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348336552"/>
+        <c:crossAx val="120001096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-BE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-BE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-BE" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Doubeling experiment (max. lengte zijde = 0.2) </a:t>
+            </a:r>
+            <a:endParaRPr lang="nl-BE">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-BE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'s &lt;= 0,2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Algoritme1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'s &lt;= 0,2'!$A$2:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'s &lt;= 0,2'!$B$2:$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>5.9249999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6248000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.4178999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.36109599999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3944639999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2993139999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1850589999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.929355999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64.363212000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91.527500000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>299.55502100000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1506.006132</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6105.5472520000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28894.072992000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>135742.56441399999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'s &lt;= 0,2'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Algoritme2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'s &lt;= 0,2'!$A$2:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'s &lt;= 0,2'!$C$2:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>1.410793</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2718000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.6248000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.101704</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.223469</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.771177</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4325200000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0100639999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.9846940000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.022172999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36.332107999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>103.923721</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>393.32140900000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3019.2715010000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11622.362928</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>71600.533431999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'s &lt;= 0,2'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Algoritme3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'s &lt;= 0,2'!$A$2:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'s &lt;= 0,2'!$D$2:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>1.253571</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2778999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19594300000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.218337</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61815500000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8745259999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3564530000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9609229999999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.7134169999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.180972000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68.046481</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>169.24192300000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>580.501485</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2943.1852749999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17320.177598999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>93547.987473999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="353032608"/>
+        <c:axId val="353034568"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="353032608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-BE"/>
+                  <a:t>Aantal rechthoeken</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-BE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="353034568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="353034568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-BE"/>
+                  <a:t>Tijd</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nl-BE" baseline="0"/>
+                  <a:t> in miliseconden</a:t>
+                </a:r>
+                <a:endParaRPr lang="nl-BE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-BE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="353032608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2162,48 +2859,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8192</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2213,48 +2868,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>4.8724999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.1363999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.168628</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.26247799999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.99839199999999995</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.2498670000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13.197941999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>39.287708000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16.915521999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44.288040000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>232.675746</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>719.36715600000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3616.9899890000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>25021.587320999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2304,48 +2917,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8192</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2355,48 +2926,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>1.455031</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.3491999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.163637</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.239428</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.75213399999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.1842050000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.3604909999999997</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>22.270868</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>22.238222</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>24.209389000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>130.66936999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>889.46861200000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2740.3895769999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14273.761823999999</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2446,48 +2975,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8192</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2497,48 +2984,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>2.3989180000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.6182000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.94386199999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.04775</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.7222439999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>20.027664000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>34.721263999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>90.492977999999994</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>165.07508000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100.277074</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>375.95076599999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1473.214066</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6566.0274239999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>38077.786604000001</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2552,11 +2997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="348337728"/>
-        <c:axId val="348332240"/>
+        <c:axId val="358811976"/>
+        <c:axId val="358813544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="348337728"/>
+        <c:axId val="358811976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2613,12 +3058,12 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348332240"/>
+        <c:crossAx val="358813544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="348332240"/>
+        <c:axId val="358813544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2676,7 +3121,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348337728"/>
+        <c:crossAx val="358811976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3020,11 +3465,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="346373960"/>
-        <c:axId val="346376704"/>
+        <c:axId val="358812368"/>
+        <c:axId val="358813936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="346373960"/>
+        <c:axId val="358812368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3137,12 +3582,12 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346376704"/>
+        <c:crossAx val="358813936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="346376704"/>
+        <c:axId val="358813936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3261,7 +3706,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346373960"/>
+        <c:crossAx val="358812368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6126,16 +6571,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>335634</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>88604</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>530388</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>32074</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>135920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6161,16 +6606,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6196,16 +6641,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6562,8 +7007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScale="86" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6586,7 +7031,245 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5.5516999999999997E-2</v>
+      </c>
+      <c r="C2">
+        <v>1.284362</v>
+      </c>
+      <c r="D2">
+        <v>1.2829630000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>7.6510999999999996E-2</v>
+      </c>
+      <c r="C3">
+        <v>6.7646999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>5.9715999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>5.9249000000000003E-2</v>
+      </c>
+      <c r="C4">
+        <v>6.2980999999999995E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.16142000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.16561899999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.12456399999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.20200899999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>0.79310400000000003</v>
+      </c>
+      <c r="C6">
+        <v>0.22673399999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.50198900000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>1.2871619999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.29065000000000002</v>
+      </c>
+      <c r="D7">
+        <v>0.74785000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>64</v>
+      </c>
+      <c r="B8">
+        <v>4.1092139999999997</v>
+      </c>
+      <c r="C8">
+        <v>0.63634999999999997</v>
+      </c>
+      <c r="D8">
+        <v>1.7746869999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <v>9.2961150000000004</v>
+      </c>
+      <c r="C9">
+        <v>4.2836959999999999</v>
+      </c>
+      <c r="D9">
+        <v>2.9979339999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>256</v>
+      </c>
+      <c r="B10">
+        <v>24.111768999999999</v>
+      </c>
+      <c r="C10">
+        <v>8.2044309999999996</v>
+      </c>
+      <c r="D10">
+        <v>4.2076510000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>512</v>
+      </c>
+      <c r="B11">
+        <v>45.772381000000003</v>
+      </c>
+      <c r="C11">
+        <v>2.0112190000000001</v>
+      </c>
+      <c r="D11">
+        <v>4.9634330000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1024</v>
+      </c>
+      <c r="B12">
+        <v>80.574263000000002</v>
+      </c>
+      <c r="C12">
+        <v>3.6268189999999998</v>
+      </c>
+      <c r="D12">
+        <v>7.2643680000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2048</v>
+      </c>
+      <c r="B13">
+        <v>205.43500399999999</v>
+      </c>
+      <c r="C13">
+        <v>7.0782220000000002</v>
+      </c>
+      <c r="D13">
+        <v>12.793704999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4096</v>
+      </c>
+      <c r="B14">
+        <v>820.38240699999994</v>
+      </c>
+      <c r="C14">
+        <v>11.974940999999999</v>
+      </c>
+      <c r="D14">
+        <v>21.557507999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>8192</v>
+      </c>
+      <c r="B15">
+        <v>3289.07998</v>
+      </c>
+      <c r="C15">
+        <v>31.238512</v>
+      </c>
+      <c r="D15">
+        <v>24.914204000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16384</v>
+      </c>
+      <c r="B16">
+        <v>15940.149552000001</v>
+      </c>
+      <c r="C16">
+        <v>102.424753</v>
+      </c>
+      <c r="D16">
+        <v>65.278081</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>32768</v>
+      </c>
+      <c r="B17">
+        <v>67381.763546999995</v>
+      </c>
+      <c r="C17">
+        <v>460.93494900000002</v>
+      </c>
+      <c r="D17">
+        <v>225.832246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>65536</v>
+      </c>
+      <c r="B18">
+        <v>285255.70148599998</v>
+      </c>
+      <c r="C18">
+        <v>1555.753831</v>
+      </c>
+      <c r="D18">
+        <v>747.09443899999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>4</v>
       </c>
@@ -6599,10 +7282,330 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5.645E-2</v>
+      </c>
+      <c r="C2">
+        <v>1.794281</v>
+      </c>
+      <c r="D2">
+        <v>34.192126000000002</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5.6451000000000001E-2</v>
+      </c>
+      <c r="C3">
+        <v>4.6186999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>6.2981999999999996E-2</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3.0324E-2</v>
+      </c>
+      <c r="C4">
+        <v>3.0324E-2</v>
+      </c>
+      <c r="D4">
+        <v>9.4239000000000003E-2</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.15068999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.18474699999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.42687700000000001</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>0.67367200000000005</v>
+      </c>
+      <c r="C6">
+        <v>0.28271800000000002</v>
+      </c>
+      <c r="D6">
+        <v>0.57663399999999998</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>1.0622929999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.39375300000000002</v>
+      </c>
+      <c r="D7">
+        <v>1.0319689999999999</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>64</v>
+      </c>
+      <c r="B8">
+        <v>3.6431480000000001</v>
+      </c>
+      <c r="C8">
+        <v>1.137872</v>
+      </c>
+      <c r="D8">
+        <v>5.5125409999999997</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>128</v>
+      </c>
+      <c r="B9">
+        <v>7.9315090000000001</v>
+      </c>
+      <c r="C9">
+        <v>1.9076489999999999</v>
+      </c>
+      <c r="D9">
+        <v>6.5906960000000003</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>256</v>
+      </c>
+      <c r="B10">
+        <v>27.048589</v>
+      </c>
+      <c r="C10">
+        <v>6.9419950000000004</v>
+      </c>
+      <c r="D10">
+        <v>6.9849160000000001</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>512</v>
+      </c>
+      <c r="B11">
+        <v>69.110174000000001</v>
+      </c>
+      <c r="C11">
+        <v>9.6436820000000001</v>
+      </c>
+      <c r="D11">
+        <v>14.023949</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1024</v>
+      </c>
+      <c r="B12">
+        <v>76.222920000000002</v>
+      </c>
+      <c r="C12">
+        <v>8.8930319999999998</v>
+      </c>
+      <c r="D12">
+        <v>18.467199999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2048</v>
+      </c>
+      <c r="B13">
+        <v>258.82211899999999</v>
+      </c>
+      <c r="C13">
+        <v>29.101796</v>
+      </c>
+      <c r="D13">
+        <v>45.625889000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4096</v>
+      </c>
+      <c r="B14">
+        <v>1073.4199960000001</v>
+      </c>
+      <c r="C14">
+        <v>128.773077</v>
+      </c>
+      <c r="D14">
+        <v>178.02485300000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>8192</v>
+      </c>
+      <c r="B15">
+        <v>4403.0896540000003</v>
+      </c>
+      <c r="C15">
+        <v>686.64916300000004</v>
+      </c>
+      <c r="D15">
+        <v>660.72211700000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16384</v>
+      </c>
+      <c r="B16">
+        <v>22048.870620000002</v>
+      </c>
+      <c r="C16">
+        <v>2393.8336610000001</v>
+      </c>
+      <c r="D16">
+        <v>3076.5924129999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>32768</v>
+      </c>
+      <c r="B17">
+        <v>84398.026849999995</v>
+      </c>
+      <c r="C17">
+        <v>13215.184121</v>
+      </c>
+      <c r="D17">
+        <v>16846.653752999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="B2" sqref="B2:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6630,13 +7633,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>4.7223000000000001E-2</v>
+        <v>5.9249999999999997E-2</v>
       </c>
       <c r="C2" s="2">
-        <v>1.427926</v>
+        <v>1.410793</v>
       </c>
       <c r="D2" s="2">
-        <v>2.3958879999999998</v>
+        <v>1.253571</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -6644,13 +7647,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>6.9347000000000006E-2</v>
+        <v>6.6248000000000001E-2</v>
       </c>
       <c r="C3" s="2">
-        <v>5.5888E-2</v>
+        <v>5.2718000000000001E-2</v>
       </c>
       <c r="D3" s="2">
-        <v>4.6593000000000002E-2</v>
+        <v>7.2778999999999996E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -6658,13 +7661,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>5.9225E-2</v>
+        <v>7.4178999999999995E-2</v>
       </c>
       <c r="C4" s="2">
-        <v>6.8627999999999995E-2</v>
+        <v>6.6248000000000001E-2</v>
       </c>
       <c r="D4" s="2">
-        <v>0.30030099999999998</v>
+        <v>0.19594300000000001</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -6672,13 +7675,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>0.35874600000000001</v>
+        <v>0.11849999999999999</v>
       </c>
       <c r="C5" s="2">
-        <v>0.25318400000000002</v>
+        <v>0.101704</v>
       </c>
       <c r="D5" s="2">
-        <v>0.67792300000000005</v>
+        <v>0.218337</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -6686,13 +7689,13 @@
         <v>16</v>
       </c>
       <c r="B6" s="2">
-        <v>0.77075300000000002</v>
+        <v>0.36109599999999997</v>
       </c>
       <c r="C6" s="2">
-        <v>0.46081499999999997</v>
+        <v>0.223469</v>
       </c>
       <c r="D6" s="2">
-        <v>1.8269759999999999</v>
+        <v>0.61815500000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -6700,13 +7703,13 @@
         <v>32</v>
       </c>
       <c r="B7" s="2">
-        <v>3.4476689999999999</v>
+        <v>1.3944639999999999</v>
       </c>
       <c r="C7" s="2">
-        <v>1.766035</v>
+        <v>0.771177</v>
       </c>
       <c r="D7" s="2">
-        <v>8.3838950000000008</v>
+        <v>1.8745259999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -6714,13 +7717,13 @@
         <v>64</v>
       </c>
       <c r="B8" s="2">
-        <v>16.724685999999998</v>
+        <v>3.2993139999999999</v>
       </c>
       <c r="C8" s="2">
-        <v>3.5092669999999999</v>
+        <v>4.4325200000000002</v>
       </c>
       <c r="D8" s="2">
-        <v>16.409811999999999</v>
+        <v>2.3564530000000001</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -6728,13 +7731,13 @@
         <v>128</v>
       </c>
       <c r="B9" s="2">
-        <v>64.328180000000003</v>
+        <v>7.1850589999999999</v>
       </c>
       <c r="C9" s="2">
-        <v>17.058319000000001</v>
+        <v>3.0100639999999999</v>
       </c>
       <c r="D9" s="2">
-        <v>113.157793</v>
+        <v>9.9609229999999993</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -6742,13 +7745,13 @@
         <v>256</v>
       </c>
       <c r="B10" s="2">
-        <v>45.292262000000001</v>
+        <v>23.929355999999999</v>
       </c>
       <c r="C10" s="2">
-        <v>16.253195000000002</v>
+        <v>7.9846940000000002</v>
       </c>
       <c r="D10" s="2">
-        <v>82.311852999999999</v>
+        <v>8.7134169999999997</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -6756,13 +7759,13 @@
         <v>512</v>
       </c>
       <c r="B11" s="2">
-        <v>28.154897999999999</v>
+        <v>64.363212000000004</v>
       </c>
       <c r="C11" s="2">
-        <v>14.791833</v>
+        <v>22.022172999999999</v>
       </c>
       <c r="D11" s="2">
-        <v>65.254551000000006</v>
+        <v>17.180972000000001</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -6770,13 +7773,13 @@
         <v>1024</v>
       </c>
       <c r="B12" s="2">
-        <v>89.458753999999999</v>
+        <v>91.527500000000003</v>
       </c>
       <c r="C12" s="2">
-        <v>35.258977999999999</v>
+        <v>36.332107999999998</v>
       </c>
       <c r="D12" s="2">
-        <v>109.60528600000001</v>
+        <v>68.046481</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -6784,13 +7787,13 @@
         <v>2048</v>
       </c>
       <c r="B13" s="2">
-        <v>409.24207899999999</v>
+        <v>299.55502100000001</v>
       </c>
       <c r="C13" s="2">
-        <v>158.16474700000001</v>
+        <v>103.923721</v>
       </c>
       <c r="D13" s="2">
-        <v>342.60131000000001</v>
+        <v>169.24192300000001</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -6798,13 +7801,13 @@
         <v>4096</v>
       </c>
       <c r="B14" s="2">
-        <v>1698.683477</v>
+        <v>1506.006132</v>
       </c>
       <c r="C14" s="2">
-        <v>845.33772199999999</v>
+        <v>393.32140900000002</v>
       </c>
       <c r="D14" s="2">
-        <v>1600.68336</v>
+        <v>580.501485</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -6812,13 +7815,13 @@
         <v>8192</v>
       </c>
       <c r="B15" s="2">
-        <v>8778.2531400000007</v>
+        <v>6105.5472520000003</v>
       </c>
       <c r="C15" s="2">
-        <v>2508.9897179999998</v>
+        <v>3019.2715010000002</v>
       </c>
       <c r="D15" s="2">
-        <v>6551.8527519999998</v>
+        <v>2943.1852749999998</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -6826,13 +7829,13 @@
         <v>16384</v>
       </c>
       <c r="B16" s="2">
-        <v>36192.314450999998</v>
+        <v>28894.072992000001</v>
       </c>
       <c r="C16" s="2">
-        <v>20610.072639000002</v>
+        <v>11622.362928</v>
       </c>
       <c r="D16" s="2">
-        <v>32770.112476000002</v>
+        <v>17320.177598999999</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -6840,13 +7843,13 @@
         <v>32768</v>
       </c>
       <c r="B17">
-        <v>231158.01998899999</v>
+        <v>135742.56441399999</v>
       </c>
       <c r="C17">
-        <v>94613.954494000005</v>
+        <v>71600.533431999997</v>
       </c>
       <c r="D17">
-        <v>160632.83349300001</v>
+        <v>93547.987473999994</v>
       </c>
     </row>
   </sheetData>
@@ -6856,128 +7859,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="A2:E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6994,202 +7881,6 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>4.8724999999999997E-2</v>
-      </c>
-      <c r="C2">
-        <v>1.455031</v>
-      </c>
-      <c r="D2">
-        <v>2.3989180000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>7.1363999999999997E-2</v>
-      </c>
-      <c r="C3">
-        <v>5.3491999999999998E-2</v>
-      </c>
-      <c r="D3">
-        <v>4.6182000000000001E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>0.168628</v>
-      </c>
-      <c r="C4">
-        <v>0.163637</v>
-      </c>
-      <c r="D4">
-        <v>0.94386199999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>0.26247799999999999</v>
-      </c>
-      <c r="C5">
-        <v>0.239428</v>
-      </c>
-      <c r="D5">
-        <v>1.04775</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>0.99839199999999995</v>
-      </c>
-      <c r="C6">
-        <v>0.75213399999999997</v>
-      </c>
-      <c r="D6">
-        <v>3.7222439999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>32</v>
-      </c>
-      <c r="B7">
-        <v>5.2498670000000001</v>
-      </c>
-      <c r="C7">
-        <v>4.1842050000000004</v>
-      </c>
-      <c r="D7">
-        <v>20.027664000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>64</v>
-      </c>
-      <c r="B8">
-        <v>13.197941999999999</v>
-      </c>
-      <c r="C8">
-        <v>7.3604909999999997</v>
-      </c>
-      <c r="D8">
-        <v>34.721263999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>128</v>
-      </c>
-      <c r="B9">
-        <v>39.287708000000002</v>
-      </c>
-      <c r="C9">
-        <v>22.270868</v>
-      </c>
-      <c r="D9">
-        <v>90.492977999999994</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>256</v>
-      </c>
-      <c r="B10">
-        <v>16.915521999999999</v>
-      </c>
-      <c r="C10">
-        <v>22.238222</v>
-      </c>
-      <c r="D10">
-        <v>165.07508000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>512</v>
-      </c>
-      <c r="B11">
-        <v>44.288040000000002</v>
-      </c>
-      <c r="C11">
-        <v>24.209389000000002</v>
-      </c>
-      <c r="D11">
-        <v>100.277074</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1024</v>
-      </c>
-      <c r="B12">
-        <v>232.675746</v>
-      </c>
-      <c r="C12">
-        <v>130.66936999999999</v>
-      </c>
-      <c r="D12">
-        <v>375.95076599999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2048</v>
-      </c>
-      <c r="B13">
-        <v>719.36715600000002</v>
-      </c>
-      <c r="C13">
-        <v>889.46861200000001</v>
-      </c>
-      <c r="D13">
-        <v>1473.214066</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>4096</v>
-      </c>
-      <c r="B14">
-        <v>3616.9899890000002</v>
-      </c>
-      <c r="C14">
-        <v>2740.3895769999999</v>
-      </c>
-      <c r="D14">
-        <v>6566.0274239999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>8192</v>
-      </c>
-      <c r="B15">
-        <v>25021.587320999999</v>
-      </c>
-      <c r="C15">
-        <v>14273.761823999999</v>
-      </c>
-      <c r="D15">
-        <v>38077.786604000001</v>
       </c>
     </row>
   </sheetData>
@@ -7202,7 +7893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bespreking resultaten deel 1
Former-commit-id: f510b0ef3f6945895d4f922f1a9aeb6cca8d0094
</commit_message>
<xml_diff>
--- a/Tijdscomplexiteit algoritmen.xlsx
+++ b/Tijdscomplexiteit algoritmen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="s &lt;= 0,01" sheetId="5" r:id="rId1"/>
@@ -665,11 +665,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="384017008"/>
-        <c:axId val="384019752"/>
+        <c:axId val="351539712"/>
+        <c:axId val="351534224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="384017008"/>
+        <c:axId val="351539712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -781,12 +781,12 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384019752"/>
+        <c:crossAx val="351534224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="384019752"/>
+        <c:axId val="351534224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -904,7 +904,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384017008"/>
+        <c:crossAx val="351539712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1534,11 +1534,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="384013480"/>
-        <c:axId val="384012304"/>
+        <c:axId val="359089848"/>
+        <c:axId val="359084752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="384013480"/>
+        <c:axId val="359089848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,12 +1650,12 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384012304"/>
+        <c:crossAx val="359084752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="384012304"/>
+        <c:axId val="359084752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1773,7 +1773,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384013480"/>
+        <c:crossAx val="359089848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1898,7 +1898,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2404,11 +2403,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="384018184"/>
-        <c:axId val="384018576"/>
+        <c:axId val="359084360"/>
+        <c:axId val="359085536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="384018184"/>
+        <c:axId val="359084360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2454,7 +2453,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2521,12 +2519,12 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384018576"/>
+        <c:crossAx val="359085536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="384018576"/>
+        <c:axId val="359085536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2578,7 +2576,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2645,7 +2642,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384018184"/>
+        <c:crossAx val="359084360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2659,7 +2656,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3259,11 +3255,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="378125888"/>
-        <c:axId val="378122752"/>
+        <c:axId val="359089064"/>
+        <c:axId val="359088280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="378125888"/>
+        <c:axId val="359089064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3320,12 +3316,12 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="378122752"/>
+        <c:crossAx val="359088280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="378122752"/>
+        <c:axId val="359088280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3383,7 +3379,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="378125888"/>
+        <c:crossAx val="359089064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3979,11 +3975,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="378127848"/>
-        <c:axId val="378123144"/>
+        <c:axId val="359090632"/>
+        <c:axId val="359088672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="378127848"/>
+        <c:axId val="359090632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4096,12 +4092,12 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="378123144"/>
+        <c:crossAx val="359088672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="378123144"/>
+        <c:axId val="359088672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4220,7 +4216,7 @@
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="378127848"/>
+        <c:crossAx val="359090632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7225,16 +7221,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8377,8 +8373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8617,7 +8613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>